<commit_message>
Inclusao de mais um histograma no excel
</commit_message>
<xml_diff>
--- a/Analyze/Mapa Planilha de PADs - Silmara.xlsx
+++ b/Analyze/Mapa Planilha de PADs - Silmara.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruhan\Documents\TCC\Analyze\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Medicao Silmara" sheetId="5" r:id="rId1"/>
@@ -948,9 +948,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -972,6 +969,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -987,6 +987,1332 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Histograma</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> de Defeitos mais recorrentes nos PAds</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="17"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="18"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="29"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="31"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="32"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="36"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="42"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="43"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="44"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'PARETO DEFEITOS'!$B$5:$B$50</c:f>
+              <c:strCache>
+                <c:ptCount val="46"/>
+                <c:pt idx="0">
+                  <c:v>Defeito -  esquecer de citar item faltante no projeto básico ou no estudo técnic</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> FALTA DE ESTUDOS PRELIMINARES </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>  TÍTULO DO PROJETO</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>  NÚMERO DO PAD / FALTA DO DOC. COMO MINUTA</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>  GESTOR E DEMANDANTE</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>  TERMO DE OFICIALIZAÇÃO DA DEMANDA</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>  JUSTIFICATIVAS</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>  DESCRIÇÃO DO OBJETO DE FORMA CLARA,  CORRETA E</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>  FOTOS OU DESENHO PERTINENTE</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>  PREVISÃO EM PROPOSTA ORÇAMENTÁRIA</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>  PESQUISA DO OBJETO JUNTO AO MERCADO OU OUTRO</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>  PRECIFICAÇÃO E/OU COMPATIBILIDADE DOS ORÇAMENT</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>  QUADRO RESUMO CONTENDO OS PRAZOS EXIGIDOS NO P</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>  DESCRIÇÃO DA GARANTIA</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>  OBRIGAÇÕES DA CONTRATADA E OBRIGAÇÕES ESPECÍFI</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>  CRITÉRIOS DE SUSTENTABILIDADE E/OU EPIs</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>  RECEBIMENTOS PROVISÓRIO E DEFINITIVO</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>  ANEXO COM TERMO DE RECEBIMENTO PROVISÓRIO</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>  ANEXO DE ATESTADO PARA PAGAMENTO/RECEBIMENTO D</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v> CLÁUSULA DO CONTRATO OU NE (VIGÊNCIA, PRAZO DE </c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v> CLÁUSULA DO PAGAMENTO</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v> CLÁUSULA DO GESTOR E/OU FISCAL</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>  ANS - ACORDO DE NÍVEIS DE SERVIÇO</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>  SUGESTÃO DE SANÇÕES </c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>  DOCUMENTOS HABILITATÓRIOS</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>  CLÁUSULA GERAL - DISPOSIÇÕES GERAIS</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Defeito -  esquecer de citar item faltante no projeto básico ou no estudo técnic</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>FALTA DE ESTUDO TÉCNICO PRELIMINAR</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>FALTA DE FOTOS E/OU LAYOUT E/OU FIGURAS PARA MELHOR VISUALIZAÇÃO DO OBJETO/LOCAL</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>NUMERO DO PAD / FALTA DO DOC COMO MINUTA</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>IDENTIFICAÇÃO COMPLETA DA DEMANDA</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>HISTÓRICO DE CONTRATAÇÕES ANTERIORES</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>DESCRIÇÃO DO OBJETO DE FORMA CLARA E CORRETA /DETALHAMENTO</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>REQUISITOS DA CONTRATAÇÃO </c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>ALINHAMENTO AOS PLANOS DO TRE INCLUINDO SUSTENTABILIDADE/JUSTIFICATIVA</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>RELAÇÃO ENTRE A DEMANDA PREVISTA E A QUANTIDADE DE CADA ITEM</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>LEVANTAMENTO PRELIMINAR DO MERCADO/PRECIFICAÇÃO/MÉTODO DE CÁLCULO INCOMPLETO</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>JUSTIFICATIVAS PARA O PARCELAMENTO OU NÃO DO OBJETO</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>PREVISÃO EM PROPOSTA ORÇAMENTÁRIA</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>SOLUÇÕES EXISTENTES/JUSTIFICATIVAS DA ESCOLHA DO TIPO DE OBJETO</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>RESULTADOS PRETENDIDOS E/OU DOS PRAZOS</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>PROVIDÊNCIAS PARA A ADEQUAÇÃO DO AMBIENTE DO ÓRGÃO E/OU IMPACTOS DA CONTRATAÇÃO</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>DO CONTRATO/VIGÊNCIA  E ININTERRUPÇÃO SERVIÇOS</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>IDENTIFICAÇÃO E ANÁLISE DOS RISCOS </c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>DO PEDIDO PARA DECLARAÇÃO DE VIABILIDADE DA CONTRATAÇÃO</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>SISTEMÁTICAS LEGAIS / LEGISLAÇÃO APLICÁVEL AO OBJETO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'PARETO DEFEITOS'!$C$5:$C$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="46"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="335481208"/>
+        <c:axId val="335481600"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="335481208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="335481600"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="335481600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="335481208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1269,6 +2595,36 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>357673</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>13411</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>179916</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>42333</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1579,10 +2935,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="57"/>
+      <c r="C1" s="56"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
@@ -1590,14 +2946,14 @@
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="K1" s="14"/>
-      <c r="AM1" s="60" t="s">
+      <c r="AM1" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="AN1" s="60"/>
+      <c r="AN1" s="59"/>
     </row>
     <row r="2" spans="1:52" ht="120" x14ac:dyDescent="0.25">
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
       <c r="D2" s="16" t="s">
         <v>45</v>
       </c>
@@ -1700,13 +3056,13 @@
       <c r="AK2" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="AM2" s="60"/>
-      <c r="AN2" s="60"/>
-      <c r="AO2" s="58"/>
+      <c r="AM2" s="59"/>
+      <c r="AN2" s="59"/>
+      <c r="AO2" s="57"/>
     </row>
     <row r="3" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
       <c r="D3" s="16" t="s">
         <v>30</v>
       </c>
@@ -1803,13 +3159,13 @@
       <c r="AI3" s="16"/>
       <c r="AJ3" s="16"/>
       <c r="AK3" s="16"/>
-      <c r="AM3" s="60"/>
-      <c r="AN3" s="60"/>
-      <c r="AO3" s="58"/>
+      <c r="AM3" s="59"/>
+      <c r="AN3" s="59"/>
+      <c r="AO3" s="57"/>
     </row>
     <row r="4" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
       <c r="D4" s="15" t="s">
         <v>7</v>
       </c>
@@ -1912,9 +3268,9 @@
       <c r="AK4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="AM4" s="60"/>
-      <c r="AN4" s="60"/>
-      <c r="AO4" s="58"/>
+      <c r="AM4" s="59"/>
+      <c r="AN4" s="59"/>
+      <c r="AO4" s="57"/>
     </row>
     <row r="5" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
@@ -1926,9 +3282,9 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="AM5" s="60"/>
-      <c r="AN5" s="60"/>
-      <c r="AO5" s="59"/>
+      <c r="AM5" s="59"/>
+      <c r="AN5" s="59"/>
+      <c r="AO5" s="58"/>
       <c r="AX5" t="s">
         <v>8</v>
       </c>
@@ -1937,7 +3293,7 @@
       </c>
     </row>
     <row r="6" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="19">
@@ -1990,14 +3346,14 @@
       <c r="AI6" s="5"/>
       <c r="AJ6" s="5"/>
       <c r="AK6" s="7"/>
-      <c r="AM6" s="53">
+      <c r="AM6" s="60">
         <f>COUNTIF(D6:AK6,"X")</f>
         <v>0</v>
       </c>
-      <c r="AN6" s="53"/>
+      <c r="AN6" s="60"/>
     </row>
     <row r="7" spans="1:52" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="20">
         <v>2</v>
       </c>
@@ -2048,14 +3404,14 @@
       <c r="AI7" s="8"/>
       <c r="AJ7" s="8"/>
       <c r="AK7" s="10"/>
-      <c r="AM7" s="53">
+      <c r="AM7" s="60">
         <f>COUNTIF(D7:AK7,"X")</f>
         <v>0</v>
       </c>
-      <c r="AN7" s="53"/>
+      <c r="AN7" s="60"/>
     </row>
     <row r="8" spans="1:52" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="56"/>
+      <c r="A8" s="55"/>
       <c r="B8" s="21">
         <v>3</v>
       </c>
@@ -2096,11 +3452,11 @@
       <c r="AI8" s="11"/>
       <c r="AJ8" s="11"/>
       <c r="AK8" s="13"/>
-      <c r="AM8" s="53">
+      <c r="AM8" s="60">
         <f>COUNTIF(D8:AK8,"X")</f>
         <v>0</v>
       </c>
-      <c r="AN8" s="53"/>
+      <c r="AN8" s="60"/>
     </row>
     <row r="9" spans="1:52" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="29"/>
@@ -2146,11 +3502,11 @@
       <c r="AI9" s="8"/>
       <c r="AJ9" s="8"/>
       <c r="AK9" s="10"/>
-      <c r="AM9" s="53">
+      <c r="AM9" s="60">
         <f t="shared" ref="AM9:AM10" si="0">COUNTIF(D9:AK9,"X")</f>
         <v>1</v>
       </c>
-      <c r="AN9" s="53"/>
+      <c r="AN9" s="60"/>
     </row>
     <row r="10" spans="1:52" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29"/>
@@ -2222,14 +3578,14 @@
       <c r="AI10" s="8"/>
       <c r="AJ10" s="8"/>
       <c r="AK10" s="10"/>
-      <c r="AM10" s="53">
+      <c r="AM10" s="60">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AN10" s="53"/>
+      <c r="AN10" s="60"/>
     </row>
     <row r="11" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="55" t="s">
+      <c r="A11" s="54" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="20">
@@ -2291,14 +3647,14 @@
       </c>
       <c r="AG11" s="47"/>
       <c r="AK11" s="10"/>
-      <c r="AM11" s="53">
+      <c r="AM11" s="60">
         <f t="shared" ref="AM11:AM42" si="1">COUNTIF(D11:AK11,"X")</f>
         <v>11</v>
       </c>
-      <c r="AN11" s="53"/>
+      <c r="AN11" s="60"/>
     </row>
     <row r="12" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="54"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="20">
         <v>7</v>
       </c>
@@ -2343,14 +3699,14 @@
         <v>119</v>
       </c>
       <c r="AK12" s="10"/>
-      <c r="AM12" s="53">
+      <c r="AM12" s="60">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="AN12" s="53"/>
+      <c r="AN12" s="60"/>
     </row>
     <row r="13" spans="1:52" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="54"/>
+      <c r="A13" s="53"/>
       <c r="B13" s="20">
         <v>8</v>
       </c>
@@ -2413,14 +3769,14 @@
         <v>0</v>
       </c>
       <c r="AK13" s="10"/>
-      <c r="AM13" s="53">
+      <c r="AM13" s="60">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="AN13" s="53"/>
+      <c r="AN13" s="60"/>
     </row>
     <row r="14" spans="1:52" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
+      <c r="A14" s="53"/>
       <c r="B14" s="20">
         <v>9</v>
       </c>
@@ -2464,14 +3820,14 @@
         <v>0</v>
       </c>
       <c r="AK14" s="10"/>
-      <c r="AM14" s="53">
+      <c r="AM14" s="60">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="AN14" s="53"/>
+      <c r="AN14" s="60"/>
     </row>
     <row r="15" spans="1:52" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="54"/>
+      <c r="A15" s="53"/>
       <c r="B15" s="20">
         <v>10</v>
       </c>
@@ -2510,14 +3866,14 @@
         <v>0</v>
       </c>
       <c r="AK15" s="10"/>
-      <c r="AM15" s="53">
+      <c r="AM15" s="60">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="AN15" s="53"/>
+      <c r="AN15" s="60"/>
     </row>
     <row r="16" spans="1:52" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
+      <c r="A16" s="53"/>
       <c r="B16" s="20">
         <v>11</v>
       </c>
@@ -2555,14 +3911,14 @@
         <v>0</v>
       </c>
       <c r="AK16" s="10"/>
-      <c r="AM16" s="53">
+      <c r="AM16" s="60">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="AN16" s="53"/>
+      <c r="AN16" s="60"/>
     </row>
     <row r="17" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
+      <c r="A17" s="53"/>
       <c r="B17" s="20">
         <v>12</v>
       </c>
@@ -2601,14 +3957,14 @@
         <v>0</v>
       </c>
       <c r="AK17" s="10"/>
-      <c r="AM17" s="53">
+      <c r="AM17" s="60">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="AN17" s="53"/>
+      <c r="AN17" s="60"/>
     </row>
     <row r="18" spans="1:48" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="54"/>
+      <c r="A18" s="53"/>
       <c r="B18" s="20">
         <v>13</v>
       </c>
@@ -2653,14 +4009,14 @@
         <v>0</v>
       </c>
       <c r="AK18" s="10"/>
-      <c r="AM18" s="53">
+      <c r="AM18" s="60">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="AN18" s="53"/>
+      <c r="AN18" s="60"/>
     </row>
     <row r="19" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="54"/>
+      <c r="A19" s="53"/>
       <c r="B19" s="20">
         <v>14</v>
       </c>
@@ -2693,14 +4049,14 @@
         <v>0</v>
       </c>
       <c r="AK19" s="10"/>
-      <c r="AM19" s="53">
+      <c r="AM19" s="60">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="AN19" s="53"/>
+      <c r="AN19" s="60"/>
     </row>
     <row r="20" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="54"/>
+      <c r="A20" s="53"/>
       <c r="B20" s="20">
         <v>15</v>
       </c>
@@ -2739,14 +4095,14 @@
         <v>0</v>
       </c>
       <c r="AK20" s="10"/>
-      <c r="AM20" s="53">
+      <c r="AM20" s="60">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="AN20" s="53"/>
+      <c r="AN20" s="60"/>
     </row>
     <row r="21" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="54"/>
+      <c r="A21" s="53"/>
       <c r="B21" s="20">
         <v>16</v>
       </c>
@@ -2789,14 +4145,14 @@
         <v>0</v>
       </c>
       <c r="AK21" s="10"/>
-      <c r="AM21" s="53">
+      <c r="AM21" s="60">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="AN21" s="53"/>
+      <c r="AN21" s="60"/>
     </row>
     <row r="22" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="54"/>
+      <c r="A22" s="53"/>
       <c r="B22" s="20">
         <v>17</v>
       </c>
@@ -2813,14 +4169,14 @@
       </c>
       <c r="V22" s="36"/>
       <c r="AK22" s="10"/>
-      <c r="AM22" s="53">
+      <c r="AM22" s="60">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AN22" s="53"/>
+      <c r="AN22" s="60"/>
     </row>
     <row r="23" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="54"/>
+      <c r="A23" s="53"/>
       <c r="B23" s="20">
         <v>18</v>
       </c>
@@ -2843,14 +4199,14 @@
       </c>
       <c r="V23" s="36"/>
       <c r="AK23" s="10"/>
-      <c r="AM23" s="53">
+      <c r="AM23" s="60">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="AN23" s="53"/>
+      <c r="AN23" s="60"/>
     </row>
     <row r="24" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="54"/>
+      <c r="A24" s="53"/>
       <c r="B24" s="20">
         <v>19</v>
       </c>
@@ -2901,14 +4257,14 @@
         <v>0</v>
       </c>
       <c r="AK24" s="10"/>
-      <c r="AM24" s="53">
+      <c r="AM24" s="60">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="AN24" s="53"/>
+      <c r="AN24" s="60"/>
     </row>
     <row r="25" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="54"/>
+      <c r="A25" s="53"/>
       <c r="B25" s="20">
         <v>20</v>
       </c>
@@ -2956,18 +4312,18 @@
         <v>0</v>
       </c>
       <c r="AK25" s="10"/>
-      <c r="AM25" s="53">
+      <c r="AM25" s="60">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="AN25" s="53"/>
+      <c r="AN25" s="60"/>
       <c r="AV25" s="9">
         <f>COUNTIF(D25:J25,"X")</f>
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="54"/>
+      <c r="A26" s="53"/>
       <c r="B26" s="20">
         <v>21</v>
       </c>
@@ -3015,18 +4371,18 @@
         <v>0</v>
       </c>
       <c r="AK26" s="10"/>
-      <c r="AM26" s="53">
+      <c r="AM26" s="60">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="AN26" s="53"/>
+      <c r="AN26" s="60"/>
       <c r="AV26" s="9">
         <f>COUNTIF(D26:J26,"X")</f>
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="54"/>
+      <c r="A27" s="53"/>
       <c r="B27" s="20">
         <v>22</v>
       </c>
@@ -3067,15 +4423,15 @@
         <v>0</v>
       </c>
       <c r="AK27" s="10"/>
-      <c r="AM27" s="53">
+      <c r="AM27" s="60">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="AN27" s="53"/>
+      <c r="AN27" s="60"/>
       <c r="AV27" s="9"/>
     </row>
     <row r="28" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="54"/>
+      <c r="A28" s="53"/>
       <c r="B28" s="20">
         <v>23</v>
       </c>
@@ -3089,18 +4445,18 @@
       <c r="H28" s="9"/>
       <c r="V28" s="36"/>
       <c r="AK28" s="10"/>
-      <c r="AM28" s="53">
+      <c r="AM28" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AN28" s="53"/>
+      <c r="AN28" s="60"/>
       <c r="AV28" s="9">
         <f>COUNTIF(D28:J28,"X")</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:48" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="56"/>
+      <c r="A29" s="55"/>
       <c r="B29" s="20"/>
       <c r="C29" s="25"/>
       <c r="D29" s="9"/>
@@ -3110,15 +4466,15 @@
       <c r="H29" s="9"/>
       <c r="V29" s="36"/>
       <c r="AK29" s="10"/>
-      <c r="AM29" s="53">
+      <c r="AM29" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AN29" s="53"/>
+      <c r="AN29" s="60"/>
       <c r="AV29" s="9"/>
     </row>
     <row r="30" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="55" t="s">
+      <c r="A30" s="54" t="s">
         <v>3</v>
       </c>
       <c r="B30" s="19">
@@ -3169,18 +4525,18 @@
       <c r="AI30" s="5"/>
       <c r="AJ30" s="5"/>
       <c r="AK30" s="7"/>
-      <c r="AM30" s="53">
+      <c r="AM30" s="60">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AN30" s="53"/>
+      <c r="AN30" s="60"/>
       <c r="AV30" s="9">
         <f>COUNTIF(D30:J30,"X")</f>
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="54"/>
+      <c r="A31" s="53"/>
       <c r="B31" s="20">
         <v>24</v>
       </c>
@@ -3221,18 +4577,18 @@
       <c r="AI31" s="8"/>
       <c r="AJ31" s="8"/>
       <c r="AK31" s="10"/>
-      <c r="AM31" s="53">
+      <c r="AM31" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AN31" s="53"/>
+      <c r="AN31" s="60"/>
       <c r="AV31" s="9">
         <f>COUNTIF(D31:J31,"X")</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="54"/>
+      <c r="A32" s="53"/>
       <c r="B32" s="20">
         <v>25</v>
       </c>
@@ -3273,18 +4629,18 @@
       <c r="AI32" s="8"/>
       <c r="AJ32" s="8"/>
       <c r="AK32" s="10"/>
-      <c r="AM32" s="53">
+      <c r="AM32" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AN32" s="53"/>
+      <c r="AN32" s="60"/>
       <c r="AV32" s="9">
         <f>COUNTIF(D32:J32,"X")</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:48" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="56"/>
+      <c r="A33" s="55"/>
       <c r="B33" s="21">
         <v>26</v>
       </c>
@@ -3325,18 +4681,18 @@
       <c r="AI33" s="11"/>
       <c r="AJ33" s="11"/>
       <c r="AK33" s="13"/>
-      <c r="AM33" s="53">
+      <c r="AM33" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AN33" s="53"/>
+      <c r="AN33" s="60"/>
       <c r="AV33" s="9">
         <f>COUNTIF(D33:J33,"X")</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="54" t="s">
+      <c r="A34" s="53" t="s">
         <v>4</v>
       </c>
       <c r="B34" s="20">
@@ -3364,18 +4720,18 @@
         <v>0</v>
       </c>
       <c r="AK34" s="10"/>
-      <c r="AM34" s="53">
+      <c r="AM34" s="60">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="AN34" s="53"/>
+      <c r="AN34" s="60"/>
       <c r="AV34" s="9">
         <f>COUNTIF(D34:J34,"X")</f>
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="54"/>
+      <c r="A35" s="53"/>
       <c r="B35" s="20">
         <v>28</v>
       </c>
@@ -3418,14 +4774,14 @@
         <v>0</v>
       </c>
       <c r="AK35" s="10"/>
-      <c r="AM35" s="53">
+      <c r="AM35" s="60">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="AN35" s="53"/>
+      <c r="AN35" s="60"/>
     </row>
     <row r="36" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="54"/>
+      <c r="A36" s="53"/>
       <c r="B36" s="20">
         <v>29</v>
       </c>
@@ -3465,14 +4821,14 @@
         <v>0</v>
       </c>
       <c r="AK36" s="10"/>
-      <c r="AM36" s="53">
+      <c r="AM36" s="60">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="AN36" s="53"/>
+      <c r="AN36" s="60"/>
     </row>
     <row r="37" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="54"/>
+      <c r="A37" s="53"/>
       <c r="B37" s="20">
         <v>30</v>
       </c>
@@ -3519,14 +4875,14 @@
         <v>0</v>
       </c>
       <c r="AK37" s="10"/>
-      <c r="AM37" s="53">
+      <c r="AM37" s="60">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="AN37" s="53"/>
+      <c r="AN37" s="60"/>
     </row>
     <row r="38" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="54"/>
+      <c r="A38" s="53"/>
       <c r="B38" s="20">
         <v>31</v>
       </c>
@@ -3543,14 +4899,14 @@
         <v>0</v>
       </c>
       <c r="AK38" s="10"/>
-      <c r="AM38" s="53">
+      <c r="AM38" s="60">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AN38" s="53"/>
+      <c r="AN38" s="60"/>
     </row>
     <row r="39" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="54"/>
+      <c r="A39" s="53"/>
       <c r="B39" s="20">
         <v>32</v>
       </c>
@@ -3586,14 +4942,14 @@
         <v>0</v>
       </c>
       <c r="AK39" s="10"/>
-      <c r="AM39" s="53">
+      <c r="AM39" s="60">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="AN39" s="53"/>
+      <c r="AN39" s="60"/>
     </row>
     <row r="40" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="54"/>
+      <c r="A40" s="53"/>
       <c r="B40" s="20">
         <v>33</v>
       </c>
@@ -3651,14 +5007,14 @@
         <v>0</v>
       </c>
       <c r="AK40" s="10"/>
-      <c r="AM40" s="53">
+      <c r="AM40" s="60">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="AN40" s="53"/>
+      <c r="AN40" s="60"/>
     </row>
     <row r="41" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="54"/>
+      <c r="A41" s="53"/>
       <c r="B41" s="20">
         <v>34</v>
       </c>
@@ -3691,14 +5047,14 @@
         <v>0</v>
       </c>
       <c r="AK41" s="10"/>
-      <c r="AM41" s="53">
+      <c r="AM41" s="60">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="AN41" s="53"/>
+      <c r="AN41" s="60"/>
     </row>
     <row r="42" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="54"/>
+      <c r="A42" s="53"/>
       <c r="B42" s="20">
         <v>35</v>
       </c>
@@ -3731,14 +5087,14 @@
         <v>0</v>
       </c>
       <c r="AK42" s="10"/>
-      <c r="AM42" s="53">
+      <c r="AM42" s="60">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="AN42" s="53"/>
+      <c r="AN42" s="60"/>
     </row>
     <row r="43" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="54"/>
+      <c r="A43" s="53"/>
       <c r="B43" s="20">
         <v>36</v>
       </c>
@@ -3763,14 +5119,14 @@
         <v>0</v>
       </c>
       <c r="AK43" s="10"/>
-      <c r="AM43" s="53">
+      <c r="AM43" s="60">
         <f t="shared" ref="AM43:AM62" si="2">COUNTIF(D43:AK43,"X")</f>
         <v>4</v>
       </c>
-      <c r="AN43" s="53"/>
+      <c r="AN43" s="60"/>
     </row>
     <row r="44" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="54"/>
+      <c r="A44" s="53"/>
       <c r="B44" s="20">
         <v>37</v>
       </c>
@@ -3798,14 +5154,14 @@
         <v>0</v>
       </c>
       <c r="AK44" s="10"/>
-      <c r="AM44" s="53">
+      <c r="AM44" s="60">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="AN44" s="53"/>
+      <c r="AN44" s="60"/>
     </row>
     <row r="45" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="54"/>
+      <c r="A45" s="53"/>
       <c r="B45" s="20">
         <v>38</v>
       </c>
@@ -3852,14 +5208,14 @@
         <v>0</v>
       </c>
       <c r="AK45" s="10"/>
-      <c r="AM45" s="53">
+      <c r="AM45" s="60">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="AN45" s="53"/>
+      <c r="AN45" s="60"/>
     </row>
     <row r="46" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="54"/>
+      <c r="A46" s="53"/>
       <c r="B46" s="20">
         <v>39</v>
       </c>
@@ -3891,14 +5247,14 @@
         <v>0</v>
       </c>
       <c r="AK46" s="10"/>
-      <c r="AM46" s="53">
+      <c r="AM46" s="60">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="AN46" s="53"/>
+      <c r="AN46" s="60"/>
     </row>
     <row r="47" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="54"/>
+      <c r="A47" s="53"/>
       <c r="B47" s="20">
         <v>40</v>
       </c>
@@ -3939,14 +5295,14 @@
         <v>0</v>
       </c>
       <c r="AK47" s="10"/>
-      <c r="AM47" s="53">
+      <c r="AM47" s="60">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="AN47" s="53"/>
+      <c r="AN47" s="60"/>
     </row>
     <row r="48" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="54"/>
+      <c r="A48" s="53"/>
       <c r="B48" s="20">
         <v>41</v>
       </c>
@@ -3968,14 +5324,14 @@
         <v>0</v>
       </c>
       <c r="AK48" s="10"/>
-      <c r="AM48" s="53">
+      <c r="AM48" s="60">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="AN48" s="53"/>
+      <c r="AN48" s="60"/>
     </row>
     <row r="49" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="54"/>
+      <c r="A49" s="53"/>
       <c r="B49" s="20">
         <v>42</v>
       </c>
@@ -4028,14 +5384,14 @@
         <v>0</v>
       </c>
       <c r="AK49" s="10"/>
-      <c r="AM49" s="53">
+      <c r="AM49" s="60">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="AN49" s="53"/>
+      <c r="AN49" s="60"/>
     </row>
     <row r="50" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="54"/>
+      <c r="A50" s="53"/>
       <c r="B50" s="20">
         <v>43</v>
       </c>
@@ -4083,14 +5439,14 @@
         <v>0</v>
       </c>
       <c r="AK50" s="10"/>
-      <c r="AM50" s="53">
+      <c r="AM50" s="60">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="AN50" s="53"/>
+      <c r="AN50" s="60"/>
     </row>
     <row r="51" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="54"/>
+      <c r="A51" s="53"/>
       <c r="B51" s="20">
         <v>44</v>
       </c>
@@ -4145,14 +5501,14 @@
         <v>0</v>
       </c>
       <c r="AK51" s="10"/>
-      <c r="AM51" s="53">
+      <c r="AM51" s="60">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="AN51" s="53"/>
+      <c r="AN51" s="60"/>
     </row>
     <row r="52" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="54"/>
+      <c r="A52" s="53"/>
       <c r="B52" s="20">
         <v>45</v>
       </c>
@@ -4195,14 +5551,14 @@
         <v>0</v>
       </c>
       <c r="AK52" s="10"/>
-      <c r="AM52" s="53">
+      <c r="AM52" s="60">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="AN52" s="53"/>
+      <c r="AN52" s="60"/>
     </row>
     <row r="53" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="54"/>
+      <c r="A53" s="53"/>
       <c r="B53" s="20">
         <v>46</v>
       </c>
@@ -4232,14 +5588,14 @@
         <v>0</v>
       </c>
       <c r="AK53" s="10"/>
-      <c r="AM53" s="53">
+      <c r="AM53" s="60">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="AN53" s="53"/>
+      <c r="AN53" s="60"/>
     </row>
     <row r="54" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="54"/>
+      <c r="A54" s="53"/>
       <c r="B54" s="20">
         <v>47</v>
       </c>
@@ -4278,14 +5634,14 @@
         <v>0</v>
       </c>
       <c r="AK54" s="10"/>
-      <c r="AM54" s="53">
+      <c r="AM54" s="60">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="AN54" s="53"/>
+      <c r="AN54" s="60"/>
     </row>
     <row r="55" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="54"/>
+      <c r="A55" s="53"/>
       <c r="B55" s="20">
         <v>48</v>
       </c>
@@ -4304,14 +5660,14 @@
       <c r="V55" s="36"/>
       <c r="W55" s="36"/>
       <c r="AK55" s="10"/>
-      <c r="AM55" s="53">
+      <c r="AM55" s="60">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AN55" s="53"/>
+      <c r="AN55" s="60"/>
     </row>
     <row r="56" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="54"/>
+      <c r="A56" s="53"/>
       <c r="B56" s="20">
         <v>49</v>
       </c>
@@ -4334,14 +5690,14 @@
         <v>0</v>
       </c>
       <c r="AK56" s="10"/>
-      <c r="AM56" s="53">
+      <c r="AM56" s="60">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="AN56" s="53"/>
+      <c r="AN56" s="60"/>
     </row>
     <row r="57" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="54"/>
+      <c r="A57" s="53"/>
       <c r="B57" s="20">
         <v>50</v>
       </c>
@@ -4365,14 +5721,14 @@
       </c>
       <c r="V57" s="36"/>
       <c r="AK57" s="10"/>
-      <c r="AM57" s="53">
+      <c r="AM57" s="60">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="AN57" s="53"/>
+      <c r="AN57" s="60"/>
     </row>
     <row r="58" spans="1:40" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="54"/>
+      <c r="A58" s="53"/>
       <c r="B58" s="20">
         <v>51</v>
       </c>
@@ -4392,14 +5748,14 @@
       </c>
       <c r="V58" s="36"/>
       <c r="AK58" s="10"/>
-      <c r="AM58" s="53">
+      <c r="AM58" s="60">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AN58" s="53"/>
+      <c r="AN58" s="60"/>
     </row>
     <row r="59" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="55" t="s">
+      <c r="A59" s="54" t="s">
         <v>5</v>
       </c>
       <c r="B59" s="19">
@@ -4451,14 +5807,14 @@
       <c r="AI59" s="5"/>
       <c r="AJ59" s="5"/>
       <c r="AK59" s="7"/>
-      <c r="AM59" s="53">
+      <c r="AM59" s="60">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="AN59" s="53"/>
+      <c r="AN59" s="60"/>
     </row>
     <row r="60" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="54"/>
+      <c r="A60" s="53"/>
       <c r="B60" s="20">
         <v>53</v>
       </c>
@@ -4502,14 +5858,14 @@
       <c r="AI60" s="8"/>
       <c r="AJ60" s="8"/>
       <c r="AK60" s="10"/>
-      <c r="AM60" s="53">
+      <c r="AM60" s="60">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AN60" s="53"/>
+      <c r="AN60" s="60"/>
     </row>
     <row r="61" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="54"/>
+      <c r="A61" s="53"/>
       <c r="B61" s="20">
         <v>54</v>
       </c>
@@ -4553,14 +5909,14 @@
       <c r="AI61" s="8"/>
       <c r="AJ61" s="8"/>
       <c r="AK61" s="10"/>
-      <c r="AM61" s="53">
+      <c r="AM61" s="60">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AN61" s="53"/>
+      <c r="AN61" s="60"/>
     </row>
     <row r="62" spans="1:40" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="56"/>
+      <c r="A62" s="55"/>
       <c r="B62" s="21">
         <v>55</v>
       </c>
@@ -4604,11 +5960,11 @@
       <c r="AI62" s="11"/>
       <c r="AJ62" s="11"/>
       <c r="AK62" s="13"/>
-      <c r="AM62" s="53">
+      <c r="AM62" s="60">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AN62" s="53"/>
+      <c r="AN62" s="60"/>
     </row>
     <row r="63" spans="1:40" x14ac:dyDescent="0.25">
       <c r="AK63" s="15"/>
@@ -4763,6 +6119,55 @@
     </row>
   </sheetData>
   <mergeCells count="65">
+    <mergeCell ref="AM9:AN9"/>
+    <mergeCell ref="AM10:AN10"/>
+    <mergeCell ref="AM62:AN62"/>
+    <mergeCell ref="AM56:AN56"/>
+    <mergeCell ref="AM57:AN57"/>
+    <mergeCell ref="AM58:AN58"/>
+    <mergeCell ref="AM59:AN59"/>
+    <mergeCell ref="AM60:AN60"/>
+    <mergeCell ref="AM61:AN61"/>
+    <mergeCell ref="AM55:AN55"/>
+    <mergeCell ref="AM45:AN45"/>
+    <mergeCell ref="AM46:AN46"/>
+    <mergeCell ref="AM47:AN47"/>
+    <mergeCell ref="AM48:AN48"/>
+    <mergeCell ref="AM49:AN49"/>
+    <mergeCell ref="AM50:AN50"/>
+    <mergeCell ref="AM52:AN52"/>
+    <mergeCell ref="AM53:AN53"/>
+    <mergeCell ref="AM54:AN54"/>
+    <mergeCell ref="AM41:AN41"/>
+    <mergeCell ref="AM42:AN42"/>
+    <mergeCell ref="AM43:AN43"/>
+    <mergeCell ref="AM44:AN44"/>
+    <mergeCell ref="AM35:AN35"/>
+    <mergeCell ref="AM36:AN36"/>
+    <mergeCell ref="AM37:AN37"/>
+    <mergeCell ref="AM38:AN38"/>
+    <mergeCell ref="AM51:AN51"/>
+    <mergeCell ref="AM29:AN29"/>
+    <mergeCell ref="AM30:AN30"/>
+    <mergeCell ref="AM31:AN31"/>
+    <mergeCell ref="AM32:AN32"/>
+    <mergeCell ref="AM34:AN34"/>
+    <mergeCell ref="AM39:AN39"/>
+    <mergeCell ref="AM40:AN40"/>
+    <mergeCell ref="AM15:AN15"/>
+    <mergeCell ref="AM16:AN16"/>
+    <mergeCell ref="AM17:AN17"/>
+    <mergeCell ref="AM18:AN18"/>
+    <mergeCell ref="AM19:AN19"/>
+    <mergeCell ref="AM20:AN20"/>
+    <mergeCell ref="AM33:AN33"/>
+    <mergeCell ref="AM22:AN22"/>
+    <mergeCell ref="AM23:AN23"/>
+    <mergeCell ref="AM24:AN24"/>
+    <mergeCell ref="AM25:AN25"/>
+    <mergeCell ref="AM26:AN26"/>
+    <mergeCell ref="AM27:AN27"/>
+    <mergeCell ref="AM28:AN28"/>
     <mergeCell ref="A34:A58"/>
     <mergeCell ref="A59:A62"/>
     <mergeCell ref="A11:A29"/>
@@ -4779,55 +6184,6 @@
     <mergeCell ref="AM12:AN12"/>
     <mergeCell ref="AM13:AN13"/>
     <mergeCell ref="AM14:AN14"/>
-    <mergeCell ref="AM39:AN39"/>
-    <mergeCell ref="AM40:AN40"/>
-    <mergeCell ref="AM15:AN15"/>
-    <mergeCell ref="AM16:AN16"/>
-    <mergeCell ref="AM17:AN17"/>
-    <mergeCell ref="AM18:AN18"/>
-    <mergeCell ref="AM19:AN19"/>
-    <mergeCell ref="AM20:AN20"/>
-    <mergeCell ref="AM33:AN33"/>
-    <mergeCell ref="AM22:AN22"/>
-    <mergeCell ref="AM23:AN23"/>
-    <mergeCell ref="AM24:AN24"/>
-    <mergeCell ref="AM25:AN25"/>
-    <mergeCell ref="AM26:AN26"/>
-    <mergeCell ref="AM27:AN27"/>
-    <mergeCell ref="AM28:AN28"/>
-    <mergeCell ref="AM29:AN29"/>
-    <mergeCell ref="AM30:AN30"/>
-    <mergeCell ref="AM31:AN31"/>
-    <mergeCell ref="AM32:AN32"/>
-    <mergeCell ref="AM34:AN34"/>
-    <mergeCell ref="AM35:AN35"/>
-    <mergeCell ref="AM36:AN36"/>
-    <mergeCell ref="AM37:AN37"/>
-    <mergeCell ref="AM38:AN38"/>
-    <mergeCell ref="AM51:AN51"/>
-    <mergeCell ref="AM52:AN52"/>
-    <mergeCell ref="AM53:AN53"/>
-    <mergeCell ref="AM54:AN54"/>
-    <mergeCell ref="AM41:AN41"/>
-    <mergeCell ref="AM42:AN42"/>
-    <mergeCell ref="AM43:AN43"/>
-    <mergeCell ref="AM44:AN44"/>
-    <mergeCell ref="AM9:AN9"/>
-    <mergeCell ref="AM10:AN10"/>
-    <mergeCell ref="AM62:AN62"/>
-    <mergeCell ref="AM56:AN56"/>
-    <mergeCell ref="AM57:AN57"/>
-    <mergeCell ref="AM58:AN58"/>
-    <mergeCell ref="AM59:AN59"/>
-    <mergeCell ref="AM60:AN60"/>
-    <mergeCell ref="AM61:AN61"/>
-    <mergeCell ref="AM55:AN55"/>
-    <mergeCell ref="AM45:AN45"/>
-    <mergeCell ref="AM46:AN46"/>
-    <mergeCell ref="AM47:AN47"/>
-    <mergeCell ref="AM48:AN48"/>
-    <mergeCell ref="AM49:AN49"/>
-    <mergeCell ref="AM50:AN50"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4838,7 +6194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
@@ -5143,8 +6499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:D50"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B3" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Corrijido local dos arquivos MInitab Projeto atualizado Planilha Silmara
</commit_message>
<xml_diff>
--- a/Analyze/Mapa Planilha de PADs - Silmara.xlsx
+++ b/Analyze/Mapa Planilha de PADs - Silmara.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Medicao Silmara" sheetId="5" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="186">
   <si>
     <t>X</t>
   </si>
@@ -452,12 +452,6 @@
     <t>NA CARTA DE CONTROLE É POSSÍVEL OBSERVAR QUE 3 PONTOS NAS AMOSTRAS 12, 15, E 23 FALHARAM</t>
   </si>
   <si>
-    <t>NO PONTO 22 VEMOS QUE HÁ UM PAD EM QUE NÃO FORAM OBSERVADOS NENHUM DEFEITOS, ESTE MERECE</t>
-  </si>
-  <si>
-    <t>ATENÇÃO PARA VERIFICARMOS SE HOUVE ALGUMA FALHA EM ANÁLISE/REVISÃO NÃO CAPTURADA.</t>
-  </si>
-  <si>
     <t>NO TESTE DE LIMITE SUPERIOR DE 3 DESVIOS PADRÃO QUE É DE 21,37 DEFEITOS</t>
   </si>
   <si>
@@ -467,9 +461,6 @@
     <t>Variável                                   Média  EP Média  DesvPad  Mínimo    Q1  Mediana     Q3  Máximo</t>
   </si>
   <si>
-    <t>QUANTIDADE DEFEITOS     11,29      1,05             5,85        0,00            7,00      11,00    15,00    24,00</t>
-  </si>
-  <si>
     <t>Defeito -  esquecer de citar item faltante no projeto básico ou no estudo técnic</t>
   </si>
   <si>
@@ -606,6 +597,21 @@
   </si>
   <si>
     <t>NÃO INSERIDO EM PARETO</t>
+  </si>
+  <si>
+    <t>deletado</t>
+  </si>
+  <si>
+    <t>QUANTIDADE DEFEITOS     11,67      1,02             5,56        3,00            7,00      11,00    15,00    24,00</t>
+  </si>
+  <si>
+    <t>ANTERIOR</t>
+  </si>
+  <si>
+    <t>NOVO</t>
+  </si>
+  <si>
+    <t>ATUALIZADA</t>
   </si>
 </sst>
 </file>
@@ -1615,11 +1621,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="335481208"/>
-        <c:axId val="335481600"/>
+        <c:axId val="105426856"/>
+        <c:axId val="107941424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="335481208"/>
+        <c:axId val="105426856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1662,7 +1668,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335481600"/>
+        <c:crossAx val="107941424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1670,7 +1676,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="335481600"/>
+        <c:axId val="107941424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1721,7 +1727,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335481208"/>
+        <c:crossAx val="105426856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2319,20 +2325,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagem 3"/>
+        <xdr:cNvPr id="7" name="Imagem 6"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2352,7 +2358,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="11849100" y="790575"/>
+          <a:off x="5562600" y="1028700"/>
           <a:ext cx="5486400" cy="3657600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2374,20 +2380,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagem 4"/>
+        <xdr:cNvPr id="8" name="Imagem 7"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2407,62 +2413,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="17649825" y="838200"/>
-          <a:ext cx="5486400" cy="3657600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Imagem 5"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5734050" y="514350"/>
+          <a:off x="11658600" y="1047750"/>
           <a:ext cx="5486400" cy="3657600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2489,15 +2440,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>472435</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>218435</xdr:colOff>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>126999</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>434576</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>180576</xdr:colOff>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2522,7 +2473,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="16379185" y="317499"/>
+          <a:off x="24570685" y="1650999"/>
           <a:ext cx="9614141" cy="6477001"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2544,15 +2495,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>323848</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>450848</xdr:colOff>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>92074</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>473851</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>600851</xdr:colOff>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2577,7 +2528,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5975348" y="282574"/>
+          <a:off x="9721848" y="1616074"/>
           <a:ext cx="9802003" cy="6607176"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2599,16 +2550,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>357673</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>13411</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>140411</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>179916</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>42333</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>203243</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>169333</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2625,6 +2576,116 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>63499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>5347</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagem 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11557000" y="9016999"/>
+          <a:ext cx="9810750" cy="6609348"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>141386</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagem 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="24955499" y="9144000"/>
+          <a:ext cx="9190137" cy="6191250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2895,9 +2956,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ67"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9:C27"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="M1" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6135,25 +6197,21 @@
     <mergeCell ref="AM48:AN48"/>
     <mergeCell ref="AM49:AN49"/>
     <mergeCell ref="AM50:AN50"/>
-    <mergeCell ref="AM52:AN52"/>
-    <mergeCell ref="AM53:AN53"/>
     <mergeCell ref="AM54:AN54"/>
     <mergeCell ref="AM41:AN41"/>
     <mergeCell ref="AM42:AN42"/>
     <mergeCell ref="AM43:AN43"/>
     <mergeCell ref="AM44:AN44"/>
+    <mergeCell ref="AM51:AN51"/>
+    <mergeCell ref="AM39:AN39"/>
+    <mergeCell ref="AM40:AN40"/>
+    <mergeCell ref="AM52:AN52"/>
+    <mergeCell ref="AM53:AN53"/>
+    <mergeCell ref="AM34:AN34"/>
     <mergeCell ref="AM35:AN35"/>
     <mergeCell ref="AM36:AN36"/>
     <mergeCell ref="AM37:AN37"/>
     <mergeCell ref="AM38:AN38"/>
-    <mergeCell ref="AM51:AN51"/>
-    <mergeCell ref="AM29:AN29"/>
-    <mergeCell ref="AM30:AN30"/>
-    <mergeCell ref="AM31:AN31"/>
-    <mergeCell ref="AM32:AN32"/>
-    <mergeCell ref="AM34:AN34"/>
-    <mergeCell ref="AM39:AN39"/>
-    <mergeCell ref="AM40:AN40"/>
     <mergeCell ref="AM15:AN15"/>
     <mergeCell ref="AM16:AN16"/>
     <mergeCell ref="AM17:AN17"/>
@@ -6168,6 +6226,10 @@
     <mergeCell ref="AM26:AN26"/>
     <mergeCell ref="AM27:AN27"/>
     <mergeCell ref="AM28:AN28"/>
+    <mergeCell ref="AM29:AN29"/>
+    <mergeCell ref="AM30:AN30"/>
+    <mergeCell ref="AM31:AN31"/>
+    <mergeCell ref="AM32:AN32"/>
     <mergeCell ref="A34:A58"/>
     <mergeCell ref="A59:A62"/>
     <mergeCell ref="A11:A29"/>
@@ -6192,10 +6254,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F37"/>
+  <dimension ref="A3:J37"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView showGridLines="0" topLeftCell="A14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6316,7 +6378,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="49" t="s">
         <v>85</v>
       </c>
@@ -6324,7 +6386,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="49" t="s">
         <v>89</v>
       </c>
@@ -6332,7 +6394,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="49" t="s">
         <v>91</v>
       </c>
@@ -6340,7 +6402,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="49" t="s">
         <v>96</v>
       </c>
@@ -6348,7 +6410,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="49" t="s">
         <v>97</v>
       </c>
@@ -6356,7 +6418,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="49" t="s">
         <v>98</v>
       </c>
@@ -6364,7 +6426,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="49" t="s">
         <v>100</v>
       </c>
@@ -6372,7 +6434,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="49" t="s">
         <v>101</v>
       </c>
@@ -6380,15 +6442,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="49" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="51" t="s">
         <v>125</v>
       </c>
-      <c r="B25" s="49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="51">
+        <v>0</v>
+      </c>
+      <c r="C25" s="52" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="49" t="s">
         <v>126</v>
       </c>
@@ -6396,7 +6461,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="49" t="s">
         <v>105</v>
       </c>
@@ -6406,8 +6471,11 @@
       <c r="F27" s="4" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="52" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="49" t="s">
         <v>106</v>
       </c>
@@ -6415,7 +6483,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="49" t="s">
         <v>111</v>
       </c>
@@ -6426,7 +6494,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="49" t="s">
         <v>112</v>
       </c>
@@ -6434,32 +6502,26 @@
         <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="49" t="s">
         <v>116</v>
       </c>
       <c r="B31" s="49">
         <v>3</v>
       </c>
-      <c r="F31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="49" t="s">
         <v>121</v>
       </c>
       <c r="B32" s="49">
         <v>6</v>
       </c>
-      <c r="F32" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="49" t="s">
         <v>122</v>
       </c>
@@ -6467,7 +6529,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="49" t="s">
         <v>127</v>
       </c>
@@ -6475,17 +6537,20 @@
         <v>3</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="J34" s="52" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F36" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
-        <v>137</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -6497,10 +6562,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:D50"/>
+  <dimension ref="A5:AL50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView showGridLines="0" topLeftCell="Y49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AL47" sqref="AL47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6509,136 +6574,142 @@
     <col min="2" max="2" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C5" s="52">
         <v>4</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C6" s="49">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C7" s="49">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="M7" s="51" t="s">
+        <v>183</v>
+      </c>
+      <c r="AL7" s="51" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C8" s="49">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C9" s="49">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C10" s="49">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C11" s="49">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C12" s="49">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C13" s="49">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="49" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C14" s="49">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="49" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C15" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C16" s="49">
         <v>5</v>
@@ -6649,7 +6720,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C17" s="49">
         <v>11</v>
@@ -6660,7 +6731,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="49" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C18" s="49">
         <v>6</v>
@@ -6671,7 +6742,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="49" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C19" s="49">
         <v>9</v>
@@ -6682,7 +6753,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="49" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C20" s="49">
         <v>2</v>
@@ -6693,7 +6764,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="49" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C21" s="49">
         <v>14</v>
@@ -6704,7 +6775,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="49" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C22" s="49">
         <v>12</v>
@@ -6715,7 +6786,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="49" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C23" s="49">
         <v>14</v>
@@ -6726,7 +6797,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="49" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C24" s="49">
         <v>10</v>
@@ -6737,7 +6808,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="49" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C25" s="49">
         <v>5</v>
@@ -6748,7 +6819,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="49" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C26" s="49">
         <v>9</v>
@@ -6759,7 +6830,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="49" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C27" s="49">
         <v>1</v>
@@ -6770,7 +6841,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="49" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C28" s="49">
         <v>3</v>
@@ -6781,7 +6852,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="49" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C29" s="49">
         <v>2</v>
@@ -6792,7 +6863,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="49" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C30" s="49">
         <v>1</v>
@@ -6803,18 +6874,18 @@
         <v>5</v>
       </c>
       <c r="B31" s="52" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C31" s="52">
         <v>3</v>
       </c>
       <c r="D31" s="51" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B32" s="49" t="s">
         <v>55</v>
@@ -6823,199 +6894,205 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A33" s="49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B33" s="49" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C33" s="49">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A34" s="49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B34" s="49" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C34" s="49">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A35" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="B35" s="49" t="s">
         <v>163</v>
-      </c>
-      <c r="B35" s="49" t="s">
-        <v>166</v>
       </c>
       <c r="C35" s="49">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A36" s="49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B36" s="49" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C36" s="49">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A37" s="49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B37" s="49" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C37" s="49">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A38" s="49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B38" s="49" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C38" s="49">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A39" s="49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B39" s="49" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C39" s="49">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A40" s="49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B40" s="49" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C40" s="49">
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A41" s="49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B41" s="49" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C41" s="49">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A42" s="49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B42" s="49" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C42" s="49">
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A43" s="49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B43" s="49" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C43" s="49">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A44" s="49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B44" s="49" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C44" s="49">
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A45" s="49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B45" s="49" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C45" s="49">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A46" s="49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B46" s="49" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C46" s="49">
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A47" s="49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B47" s="49" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C47" s="49">
         <v>13</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="AL47" s="52" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A48" s="49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B48" s="49" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C48" s="49">
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B49" s="49" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C49" s="49">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M49" s="51" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B50" s="49" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C50" s="49">
         <v>10</v>

</xml_diff>